<commit_message>
ajout dans les exports
- tags
- code étudiant
- blocs notes --> ajouter dans paramétrage
</commit_message>
<xml_diff>
--- a/src/main/resources/template/exports-xlsx/candidatures_template.xlsx
+++ b/src/main/resources/template/exports-xlsx/candidatures_template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
   <si>
     <t>&lt;jt:forEach items="${candidatures}" var="cand"&gt;${cand.candidat.compteMinima.numDossierOpiCptMin}</t>
   </si>
@@ -307,9 +307,6 @@
     <t>&lt;jt:hideCols test="${userAnnulHide}"&gt;Annulé par&lt;/jt:hideCols&gt;</t>
   </si>
   <si>
-    <t>${cand.userAnnulCand}&lt;/jt:forEach&gt;</t>
-  </si>
-  <si>
     <t>${cand.datAnnulCandStr}</t>
   </si>
   <si>
@@ -335,6 +332,21 @@
   </si>
   <si>
     <t>&lt;jt:hideCols test="${tagHide}"&gt;Tags (libellés)&lt;/jt:hideCols&gt;</t>
+  </si>
+  <si>
+    <t>${cand.candidat.compteMinima.supannEtuIdCptMin}</t>
+  </si>
+  <si>
+    <t>&lt;jt:hideCols test="${etuIdHide}"&gt;Code étudiant&lt;/jt:hideCols&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jt:hideCols test="${postItHide}"&gt;Bloc note&lt;/jt:hideCols&gt;</t>
+  </si>
+  <si>
+    <t>${cand.userAnnulCand}</t>
+  </si>
+  <si>
+    <t>${cand.blocNoteStr}&lt;/jt:forEach&gt;</t>
   </si>
 </sst>
 </file>
@@ -417,7 +429,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -431,6 +443,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -732,12 +745,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BA3"/>
+  <dimension ref="A1:BC3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q1" sqref="Q1"/>
-      <selection pane="bottomLeft" activeCell="AA12" sqref="AA12"/>
+      <selection pane="bottomLeft" activeCell="BC1" sqref="BC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -746,36 +759,37 @@
     <col min="2" max="2" width="9" style="4" customWidth="1"/>
     <col min="3" max="3" width="18.140625" style="4" customWidth="1"/>
     <col min="4" max="5" width="24.5703125" style="4" customWidth="1"/>
-    <col min="6" max="10" width="19.5703125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="15.5703125" style="4" customWidth="1"/>
-    <col min="12" max="12" width="23" style="4" customWidth="1"/>
-    <col min="13" max="21" width="15.5703125" style="4" customWidth="1"/>
-    <col min="22" max="22" width="27.85546875" style="4" customWidth="1"/>
-    <col min="23" max="23" width="20.5703125" style="4" customWidth="1"/>
-    <col min="24" max="24" width="26.140625" style="4" customWidth="1"/>
-    <col min="25" max="25" width="20.42578125" style="4" customWidth="1"/>
-    <col min="26" max="26" width="16.140625" style="4" customWidth="1"/>
-    <col min="27" max="27" width="25.140625" style="4" customWidth="1"/>
-    <col min="28" max="28" width="18.42578125" style="4" customWidth="1"/>
-    <col min="29" max="29" width="24" style="4" customWidth="1"/>
-    <col min="30" max="30" width="21" style="4" customWidth="1"/>
-    <col min="31" max="31" width="45" style="4" customWidth="1"/>
-    <col min="32" max="32" width="23.42578125" style="4" customWidth="1"/>
-    <col min="33" max="33" width="22" style="4" customWidth="1"/>
-    <col min="34" max="34" width="24.140625" style="4" customWidth="1"/>
-    <col min="35" max="35" width="22.140625" style="4" customWidth="1"/>
-    <col min="36" max="36" width="27.85546875" style="4" customWidth="1"/>
-    <col min="37" max="37" width="48.28515625" style="4" customWidth="1"/>
-    <col min="38" max="38" width="14.5703125" style="4" customWidth="1"/>
-    <col min="39" max="39" width="19.7109375" style="4" customWidth="1"/>
-    <col min="40" max="40" width="15.42578125" style="4" customWidth="1"/>
-    <col min="41" max="47" width="22" style="4" customWidth="1"/>
-    <col min="48" max="48" width="18.42578125" style="4" customWidth="1"/>
-    <col min="49" max="51" width="28.28515625" style="4" customWidth="1"/>
-    <col min="52" max="52" width="16.5703125" customWidth="1"/>
+    <col min="6" max="11" width="19.5703125" style="4" customWidth="1"/>
+    <col min="12" max="12" width="15.5703125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="23" style="4" customWidth="1"/>
+    <col min="14" max="22" width="15.5703125" style="4" customWidth="1"/>
+    <col min="23" max="23" width="27.85546875" style="4" customWidth="1"/>
+    <col min="24" max="24" width="20.5703125" style="4" customWidth="1"/>
+    <col min="25" max="25" width="26.140625" style="4" customWidth="1"/>
+    <col min="26" max="26" width="20.42578125" style="4" customWidth="1"/>
+    <col min="27" max="27" width="16.140625" style="4" customWidth="1"/>
+    <col min="28" max="28" width="25.140625" style="4" customWidth="1"/>
+    <col min="29" max="29" width="18.42578125" style="4" customWidth="1"/>
+    <col min="30" max="30" width="24" style="4" customWidth="1"/>
+    <col min="31" max="31" width="21" style="4" customWidth="1"/>
+    <col min="32" max="32" width="45" style="4" customWidth="1"/>
+    <col min="33" max="33" width="23.42578125" style="4" customWidth="1"/>
+    <col min="34" max="34" width="22" style="4" customWidth="1"/>
+    <col min="35" max="35" width="24.140625" style="4" customWidth="1"/>
+    <col min="36" max="36" width="22.140625" style="4" customWidth="1"/>
+    <col min="37" max="37" width="27.85546875" style="4" customWidth="1"/>
+    <col min="38" max="38" width="48.28515625" style="4" customWidth="1"/>
+    <col min="39" max="39" width="14.5703125" style="4" customWidth="1"/>
+    <col min="40" max="40" width="19.7109375" style="4" customWidth="1"/>
+    <col min="41" max="41" width="15.42578125" style="4" customWidth="1"/>
+    <col min="42" max="48" width="22" style="4" customWidth="1"/>
+    <col min="49" max="49" width="18.42578125" style="4" customWidth="1"/>
+    <col min="50" max="52" width="28.28515625" style="4" customWidth="1"/>
+    <col min="53" max="54" width="16.5703125" customWidth="1"/>
+    <col min="55" max="55" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:53" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:55" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -798,145 +812,151 @@
         <v>19</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="Y1" s="2" t="s">
-        <v>106</v>
-      </c>
       <c r="Z1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AA1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AH1" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AH1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="AL1" s="2" t="s">
+      <c r="AM1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="AM1" s="2" t="s">
+      <c r="AN1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="AT1" s="2" t="s">
+      <c r="AU1" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AW1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="AY1" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="AX1" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="AY1" s="2" t="s">
+      <c r="AZ1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="AZ1" s="2" t="s">
+      <c r="BA1" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="BA1" s="2" t="s">
+      <c r="BB1" s="2" t="s">
         <v>96</v>
       </c>
+      <c r="BC1" s="2" t="s">
+        <v>108</v>
+      </c>
     </row>
-    <row r="2" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -959,145 +979,151 @@
         <v>36</v>
       </c>
       <c r="H2" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="Y2" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="Z2" s="4" t="s">
+      <c r="Z2" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AB2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AC2" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AD2" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="AD2" s="4" t="s">
+      <c r="AE2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="AE2" s="4" t="s">
+      <c r="AF2" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="AF2" s="4" t="s">
+      <c r="AG2" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="AG2" s="4" t="s">
+      <c r="AH2" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="AH2" s="4" t="s">
+      <c r="AI2" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="AI2" s="4" t="s">
+      <c r="AJ2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="AJ2" s="5" t="s">
+      <c r="AK2" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="AK2" s="4" t="s">
+      <c r="AL2" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="AL2" s="4" t="s">
+      <c r="AM2" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="AM2" s="4" t="s">
+      <c r="AN2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AN2" s="5" t="s">
+      <c r="AO2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="AO2" s="4" t="s">
+      <c r="AP2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AP2" s="4" t="s">
+      <c r="AQ2" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="AQ2" s="4" t="s">
+      <c r="AR2" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="AR2" s="4" t="s">
+      <c r="AS2" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="AS2" s="4" t="s">
-        <v>102</v>
-      </c>
       <c r="AT2" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="AU2" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="AU2" s="4" t="s">
+      <c r="AV2" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="AV2" s="4" t="s">
+      <c r="AW2" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="AW2" s="4" t="s">
+      <c r="AX2" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AY2" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="AX2" s="4" t="s">
+      <c r="AZ2" s="8" t="s">
         <v>100</v>
-      </c>
-      <c r="AY2" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>98</v>
       </c>
       <c r="BA2" t="s">
         <v>97</v>
       </c>
+      <c r="BB2" t="s">
+        <v>109</v>
+      </c>
+      <c r="BC2" s="9" t="s">
+        <v>110</v>
+      </c>
     </row>
-    <row r="3" spans="1:53" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:55" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>93</v>
       </c>
@@ -1151,8 +1177,10 @@
       <c r="AW3" s="6"/>
       <c r="AX3" s="6"/>
       <c r="AY3" s="6"/>
-      <c r="AZ3" s="7"/>
+      <c r="AZ3" s="6"/>
       <c r="BA3" s="7"/>
+      <c r="BB3" s="7"/>
+      <c r="BC3" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>

<commit_message>
ajout du nom usuel dans l'export
</commit_message>
<xml_diff>
--- a/src/main/resources/template/exports-xlsx/candidatures_template.xlsx
+++ b/src/main/resources/template/exports-xlsx/candidatures_template.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
   <si>
     <t>&lt;jt:forEach items="${candidatures}" var="cand"&gt;${cand.candidat.compteMinima.numDossierOpiCptMin}</t>
   </si>
@@ -64,9 +64,6 @@
     <t>&lt;jt:hideCols test="${civiliteHide}"&gt;Civilité&lt;/jt:hideCols&gt;</t>
   </si>
   <si>
-    <t>&lt;jt:hideCols test="${nomHide}"&gt;Nom&lt;/jt:hideCols&gt;</t>
-  </si>
-  <si>
     <t>&lt;jt:hideCols test="${prenomHide}"&gt;Prénom&lt;/jt:hideCols&gt;</t>
   </si>
   <si>
@@ -353,6 +350,15 @@
   </si>
   <si>
     <t>&lt;jt:if test="${cand.lastTypeDecision.listCompRangReelTypDecCand!=null}" then="${cand.lastTypeDecision.listCompRangReelTypDecCand}"/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jt:hideCols test="${nomPatHide}"&gt;Nom patronymique&lt;/jt:hideCols&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jt:hideCols test="${nomUsuHide}"&gt;Nom usuel&lt;/jt:hideCols&gt;</t>
+  </si>
+  <si>
+    <t>${cand.candidat.nomUsuCandidat}</t>
   </si>
 </sst>
 </file>
@@ -751,7 +757,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BD3"/>
+  <dimension ref="A1:BE3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -763,39 +769,39 @@
   <cols>
     <col min="1" max="1" width="15.140625" style="4" customWidth="1"/>
     <col min="2" max="2" width="9" style="4" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="4" customWidth="1"/>
-    <col min="4" max="5" width="24.5703125" style="4" customWidth="1"/>
-    <col min="6" max="11" width="19.5703125" style="4" customWidth="1"/>
-    <col min="12" max="12" width="15.5703125" style="4" customWidth="1"/>
-    <col min="13" max="13" width="23" style="4" customWidth="1"/>
-    <col min="14" max="22" width="15.5703125" style="4" customWidth="1"/>
-    <col min="23" max="23" width="27.85546875" style="4" customWidth="1"/>
-    <col min="24" max="24" width="20.5703125" style="4" customWidth="1"/>
-    <col min="25" max="25" width="26.140625" style="4" customWidth="1"/>
-    <col min="26" max="26" width="20.42578125" style="4" customWidth="1"/>
-    <col min="27" max="27" width="16.140625" style="4" customWidth="1"/>
-    <col min="28" max="28" width="25.140625" style="4" customWidth="1"/>
-    <col min="29" max="29" width="18.42578125" style="4" customWidth="1"/>
-    <col min="30" max="30" width="24" style="4" customWidth="1"/>
-    <col min="31" max="31" width="21" style="4" customWidth="1"/>
-    <col min="32" max="32" width="45" style="4" customWidth="1"/>
-    <col min="33" max="33" width="23.42578125" style="4" customWidth="1"/>
-    <col min="34" max="34" width="22" style="4" customWidth="1"/>
-    <col min="35" max="35" width="24.140625" style="4" customWidth="1"/>
-    <col min="36" max="36" width="22.140625" style="4" customWidth="1"/>
-    <col min="37" max="37" width="27.85546875" style="4" customWidth="1"/>
-    <col min="38" max="38" width="48.28515625" style="4" customWidth="1"/>
-    <col min="39" max="39" width="14.5703125" style="4" customWidth="1"/>
-    <col min="40" max="40" width="19.7109375" style="4" customWidth="1"/>
-    <col min="41" max="41" width="15.42578125" style="4" customWidth="1"/>
-    <col min="42" max="49" width="22" style="4" customWidth="1"/>
-    <col min="50" max="50" width="18.42578125" style="4" customWidth="1"/>
-    <col min="51" max="53" width="28.28515625" style="4" customWidth="1"/>
-    <col min="54" max="55" width="16.5703125" customWidth="1"/>
-    <col min="56" max="56" width="9.140625" customWidth="1"/>
+    <col min="3" max="4" width="18.140625" style="4" customWidth="1"/>
+    <col min="5" max="6" width="24.5703125" style="4" customWidth="1"/>
+    <col min="7" max="12" width="19.5703125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="15.5703125" style="4" customWidth="1"/>
+    <col min="14" max="14" width="23" style="4" customWidth="1"/>
+    <col min="15" max="23" width="15.5703125" style="4" customWidth="1"/>
+    <col min="24" max="24" width="27.85546875" style="4" customWidth="1"/>
+    <col min="25" max="25" width="20.5703125" style="4" customWidth="1"/>
+    <col min="26" max="26" width="26.140625" style="4" customWidth="1"/>
+    <col min="27" max="27" width="20.42578125" style="4" customWidth="1"/>
+    <col min="28" max="28" width="16.140625" style="4" customWidth="1"/>
+    <col min="29" max="29" width="25.140625" style="4" customWidth="1"/>
+    <col min="30" max="30" width="18.42578125" style="4" customWidth="1"/>
+    <col min="31" max="31" width="24" style="4" customWidth="1"/>
+    <col min="32" max="32" width="21" style="4" customWidth="1"/>
+    <col min="33" max="33" width="45" style="4" customWidth="1"/>
+    <col min="34" max="34" width="23.42578125" style="4" customWidth="1"/>
+    <col min="35" max="35" width="22" style="4" customWidth="1"/>
+    <col min="36" max="36" width="24.140625" style="4" customWidth="1"/>
+    <col min="37" max="37" width="22.140625" style="4" customWidth="1"/>
+    <col min="38" max="38" width="27.85546875" style="4" customWidth="1"/>
+    <col min="39" max="39" width="48.28515625" style="4" customWidth="1"/>
+    <col min="40" max="40" width="14.5703125" style="4" customWidth="1"/>
+    <col min="41" max="41" width="19.7109375" style="4" customWidth="1"/>
+    <col min="42" max="42" width="15.42578125" style="4" customWidth="1"/>
+    <col min="43" max="50" width="22" style="4" customWidth="1"/>
+    <col min="51" max="51" width="18.42578125" style="4" customWidth="1"/>
+    <col min="52" max="54" width="28.28515625" style="4" customWidth="1"/>
+    <col min="55" max="56" width="16.5703125" customWidth="1"/>
+    <col min="57" max="57" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:56" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:57" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -803,169 +809,172 @@
         <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>61</v>
-      </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="N1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="S1" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="T1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="V1" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="W1" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="X1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="Z1" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="AA1" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="AC1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AD1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AF1" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AG1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AH1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="AN1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="AO1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AP1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="AQ1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="AR1" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="AS1" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AT1" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="AU1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="AV1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="AW1" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AX1" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="AY1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AZ1" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="BA1" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="BB1" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="BC1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="BD1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="BE1" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="T1" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="U1" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="V1" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="W1" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="X1" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="Y1" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="Z1" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="AA1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="AK1" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="AL1" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="AM1" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="AN1" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="AO1" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="AP1" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="AQ1" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AR1" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="AS1" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="AT1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AU1" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="AV1" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="AW1" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="AX1" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="AY1" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="AZ1" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="BA1" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="BB1" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="BC1" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="BD1" s="2" t="s">
-        <v>107</v>
-      </c>
     </row>
-    <row r="2" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -976,168 +985,171 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>62</v>
-      </c>
       <c r="F2" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>36</v>
-      </c>
       <c r="H2" s="3" t="s">
-        <v>105</v>
+        <v>35</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>81</v>
+        <v>104</v>
       </c>
       <c r="J2" s="3" t="s">
         <v>80</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="L2" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="M2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Q2" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="P2" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>72</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>71</v>
       </c>
       <c r="S2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="U2" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="V2" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="X2" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="Y2" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="Z2" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="Y2" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="Z2" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="AA2" s="4" t="s">
+      <c r="AA2" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="AB2" s="4" t="s">
+      <c r="AC2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="AC2" s="4" t="s">
+      <c r="AD2" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="AE2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="AF2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="AG2" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="AH2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="AI2" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AK2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="AL2" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="AM2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="AN2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="AO2" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="AP2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="AD2" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="AE2" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="AF2" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="AG2" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="AH2" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="AI2" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="AJ2" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="AK2" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="AL2" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="AM2" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="AN2" s="4" t="s">
+      <c r="AQ2" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="AR2" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="AO2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="AP2" s="4" t="s">
+      <c r="AS2" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="AT2" s="8" t="s">
+        <v>111</v>
+      </c>
+      <c r="AU2" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="AQ2" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="AR2" s="4" t="s">
-        <v>48</v>
-      </c>
-      <c r="AS2" s="8" t="s">
-        <v>112</v>
-      </c>
-      <c r="AT2" s="4" t="s">
-        <v>51</v>
-      </c>
-      <c r="AU2" s="4" t="s">
-        <v>100</v>
-      </c>
       <c r="AV2" s="4" t="s">
-        <v>88</v>
+        <v>99</v>
       </c>
       <c r="AW2" s="4" t="s">
         <v>87</v>
       </c>
       <c r="AX2" s="4" t="s">
-        <v>49</v>
+        <v>86</v>
       </c>
       <c r="AY2" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="AZ2" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="BA2" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="AZ2" s="4" t="s">
+      <c r="BB2" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="BA2" s="8" t="s">
-        <v>99</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>96</v>
-      </c>
       <c r="BC2" t="s">
+        <v>95</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>107</v>
+      </c>
+      <c r="BE2" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="BD2" s="9" t="s">
-        <v>109</v>
-      </c>
     </row>
-    <row r="3" spans="1:56" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:57" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3" s="6"/>
       <c r="C3" s="6"/>
@@ -1191,9 +1203,10 @@
       <c r="AY3" s="6"/>
       <c r="AZ3" s="6"/>
       <c r="BA3" s="6"/>
-      <c r="BB3" s="7"/>
+      <c r="BB3" s="6"/>
       <c r="BC3" s="7"/>
       <c r="BD3" s="7"/>
+      <c r="BE3" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>

<commit_message>
Saisie exo et montant suite
</commit_message>
<xml_diff>
--- a/src/main/resources/template/exports-xlsx/candidatures_template.xlsx
+++ b/src/main/resources/template/exports-xlsx/candidatures_template.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kevin\Desktop\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="2640" yWindow="765" windowWidth="18555" windowHeight="5550"/>
   </bookViews>
@@ -14,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
   <si>
     <t>&lt;jt:forEach items="${candidatures}" var="cand"&gt;${cand.candidat.compteMinima.numDossierOpiCptMin}</t>
   </si>
@@ -359,12 +364,30 @@
   </si>
   <si>
     <t>${cand.candidat.nomUsuCandidat}</t>
+  </si>
+  <si>
+    <t>&lt;jt:hideCols test="${catExoHide}"&gt;Catégorie exonération&lt;/jt:hideCols&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jt:hideCols test="${cmtExoHide}"&gt;Commentaire exonération&lt;/jt:hideCols&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jt:hideCols test="${mntChargeHide}"&gt;Montant restant à charge&lt;/jt:hideCols&gt;</t>
+  </si>
+  <si>
+    <t>${cand.catExoStr}</t>
+  </si>
+  <si>
+    <t>${cand.cmtCatExoExtCand}</t>
+  </si>
+  <si>
+    <t>${cand.mntChargeStr}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -466,6 +489,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -513,7 +539,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -548,7 +574,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -757,7 +783,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BE3"/>
+  <dimension ref="A1:BH3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -797,11 +823,14 @@
     <col min="43" max="50" width="22" style="4" customWidth="1"/>
     <col min="51" max="51" width="18.42578125" style="4" customWidth="1"/>
     <col min="52" max="54" width="28.28515625" style="4" customWidth="1"/>
-    <col min="55" max="56" width="16.5703125" customWidth="1"/>
-    <col min="57" max="57" width="9.140625" customWidth="1"/>
+    <col min="55" max="55" width="29.140625" style="4" customWidth="1"/>
+    <col min="56" max="56" width="28.28515625" style="4" customWidth="1"/>
+    <col min="57" max="57" width="26.7109375" style="4" customWidth="1"/>
+    <col min="58" max="59" width="16.5703125" customWidth="1"/>
+    <col min="60" max="60" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:60" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -965,16 +994,25 @@
         <v>34</v>
       </c>
       <c r="BC1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="BD1" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="BE1" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="BF1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="BD1" s="2" t="s">
+      <c r="BG1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="BE1" s="2" t="s">
+      <c r="BH1" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1137,17 +1175,26 @@
       <c r="BB2" s="8" t="s">
         <v>98</v>
       </c>
-      <c r="BC2" t="s">
+      <c r="BC2" s="8" t="s">
+        <v>118</v>
+      </c>
+      <c r="BD2" s="8" t="s">
+        <v>119</v>
+      </c>
+      <c r="BE2" s="8" t="s">
+        <v>120</v>
+      </c>
+      <c r="BF2" t="s">
         <v>95</v>
       </c>
-      <c r="BD2" t="s">
+      <c r="BG2" t="s">
         <v>107</v>
       </c>
-      <c r="BE2" s="9" t="s">
+      <c r="BH2" s="9" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:60" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>91</v>
       </c>
@@ -1204,9 +1251,12 @@
       <c r="AZ3" s="6"/>
       <c r="BA3" s="6"/>
       <c r="BB3" s="6"/>
-      <c r="BC3" s="7"/>
-      <c r="BD3" s="7"/>
-      <c r="BE3" s="7"/>
+      <c r="BC3" s="6"/>
+      <c r="BD3" s="6"/>
+      <c r="BE3" s="6"/>
+      <c r="BF3" s="7"/>
+      <c r="BG3" s="7"/>
+      <c r="BH3" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>

<commit_message>
Affichage des informations OPI aux gestionnaires
</commit_message>
<xml_diff>
--- a/src/main/resources/template/exports-xlsx/candidatures_template.xlsx
+++ b/src/main/resources/template/exports-xlsx/candidatures_template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
   <si>
     <t>&lt;jt:forEach items="${candidatures}" var="cand"&gt;${cand.candidat.compteMinima.numDossierOpiCptMin}</t>
   </si>
@@ -382,6 +382,18 @@
   </si>
   <si>
     <t>${cand.mntChargeStr}</t>
+  </si>
+  <si>
+    <t>&lt;jt:hideCols test="${datPassageOpiHide}"&gt;Date passage OPI&lt;/jt:hideCols&gt;</t>
+  </si>
+  <si>
+    <t>&lt;jt:hideCols test="${codOpiHide}"&gt;Code OPI&lt;/jt:hideCols&gt;</t>
+  </si>
+  <si>
+    <t>${cand.datPassageOpiStr}</t>
+  </si>
+  <si>
+    <t>${cand.codOpiStr}</t>
   </si>
 </sst>
 </file>
@@ -783,7 +795,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BH3"/>
+  <dimension ref="A1:BJ3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -826,11 +838,13 @@
     <col min="55" max="55" width="29.140625" style="4" customWidth="1"/>
     <col min="56" max="56" width="28.28515625" style="4" customWidth="1"/>
     <col min="57" max="57" width="26.7109375" style="4" customWidth="1"/>
-    <col min="58" max="59" width="16.5703125" customWidth="1"/>
-    <col min="60" max="60" width="9.140625" customWidth="1"/>
+    <col min="58" max="58" width="23" style="4" customWidth="1"/>
+    <col min="59" max="59" width="23.140625" style="4" customWidth="1"/>
+    <col min="60" max="61" width="16.5703125" customWidth="1"/>
+    <col min="62" max="62" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:60" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:62" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -1003,16 +1017,22 @@
         <v>117</v>
       </c>
       <c r="BF1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="BG1" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="BH1" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="BG1" s="2" t="s">
+      <c r="BI1" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="BH1" s="2" t="s">
+      <c r="BJ1" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1184,17 +1204,23 @@
       <c r="BE2" s="8" t="s">
         <v>120</v>
       </c>
-      <c r="BF2" t="s">
+      <c r="BF2" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="BG2" s="8" t="s">
+        <v>124</v>
+      </c>
+      <c r="BH2" t="s">
         <v>95</v>
       </c>
-      <c r="BG2" t="s">
+      <c r="BI2" t="s">
         <v>107</v>
       </c>
-      <c r="BH2" s="9" t="s">
+      <c r="BJ2" s="9" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:60" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:62" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>91</v>
       </c>
@@ -1254,9 +1280,11 @@
       <c r="BC3" s="6"/>
       <c r="BD3" s="6"/>
       <c r="BE3" s="6"/>
-      <c r="BF3" s="7"/>
-      <c r="BG3" s="7"/>
+      <c r="BF3" s="6"/>
+      <c r="BG3" s="6"/>
       <c r="BH3" s="7"/>
+      <c r="BI3" s="7"/>
+      <c r="BJ3" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>

<commit_message>
retour arriere suite reunion amue
</commit_message>
<xml_diff>
--- a/src/main/resources/template/exports-xlsx/candidatures_template.xlsx
+++ b/src/main/resources/template/exports-xlsx/candidatures_template.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
   <si>
     <t>&lt;jt:forEach items="${candidatures}" var="cand"&gt;${cand.candidat.compteMinima.numDossierOpiCptMin}</t>
   </si>
@@ -366,13 +366,7 @@
     <t>${cand.candidat.nomUsuCandidat}</t>
   </si>
   <si>
-    <t>&lt;jt:hideCols test="${catExoHide}"&gt;Catégorie exonération&lt;/jt:hideCols&gt;</t>
-  </si>
-  <si>
     <t>&lt;jt:hideCols test="${mntChargeHide}"&gt;Montant restant à charge&lt;/jt:hideCols&gt;</t>
-  </si>
-  <si>
-    <t>${cand.catExoStr}</t>
   </si>
   <si>
     <t>${cand.mntChargeStr}</t>
@@ -795,12 +789,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BJ3"/>
+  <dimension ref="A1:BI3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BA1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="Q1" sqref="Q1"/>
-      <selection pane="bottomLeft" activeCell="BD2" sqref="BD2"/>
+      <selection pane="bottomLeft"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -834,17 +828,15 @@
     <col min="42" max="42" width="15.42578125" style="4" customWidth="1"/>
     <col min="43" max="50" width="22" style="4" customWidth="1"/>
     <col min="51" max="51" width="18.42578125" style="4" customWidth="1"/>
-    <col min="52" max="54" width="28.28515625" style="4" customWidth="1"/>
-    <col min="55" max="55" width="29.140625" style="4" customWidth="1"/>
-    <col min="56" max="56" width="28.28515625" style="4" customWidth="1"/>
-    <col min="57" max="57" width="26.7109375" style="4" customWidth="1"/>
-    <col min="58" max="58" width="23" style="4" customWidth="1"/>
-    <col min="59" max="59" width="23.140625" style="4" customWidth="1"/>
-    <col min="60" max="61" width="16.5703125" customWidth="1"/>
-    <col min="62" max="62" width="9.140625" customWidth="1"/>
+    <col min="52" max="55" width="28.28515625" style="4" customWidth="1"/>
+    <col min="56" max="56" width="26.7109375" style="4" customWidth="1"/>
+    <col min="57" max="57" width="23" style="4" customWidth="1"/>
+    <col min="58" max="58" width="23.140625" style="4" customWidth="1"/>
+    <col min="59" max="60" width="16.5703125" customWidth="1"/>
+    <col min="61" max="61" width="9.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:62" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:61" s="1" customFormat="1" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>14</v>
       </c>
@@ -1008,31 +1000,28 @@
         <v>34</v>
       </c>
       <c r="BC1" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="BD1" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="BD1" s="2" t="s">
-        <v>123</v>
-      </c>
       <c r="BE1" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="BF1" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="BG1" s="2" t="s">
-        <v>120</v>
+        <v>93</v>
       </c>
       <c r="BH1" s="2" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="BI1" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="BJ1" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="2" spans="1:62" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1196,31 +1185,28 @@
         <v>98</v>
       </c>
       <c r="BC2" s="8" t="s">
-        <v>117</v>
+        <v>122</v>
       </c>
       <c r="BD2" s="8" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="BE2" s="8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="BF2" s="8" t="s">
-        <v>121</v>
-      </c>
-      <c r="BG2" s="8" t="s">
-        <v>122</v>
+        <v>120</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>95</v>
       </c>
       <c r="BH2" t="s">
-        <v>95</v>
-      </c>
-      <c r="BI2" t="s">
         <v>107</v>
       </c>
-      <c r="BJ2" s="9" t="s">
+      <c r="BI2" s="9" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="3" spans="1:62" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:61" x14ac:dyDescent="0.2">
       <c r="A3" s="6" t="s">
         <v>91</v>
       </c>
@@ -1281,10 +1267,9 @@
       <c r="BD3" s="6"/>
       <c r="BE3" s="6"/>
       <c r="BF3" s="6"/>
-      <c r="BG3" s="6"/>
+      <c r="BG3" s="7"/>
       <c r="BH3" s="7"/>
       <c r="BI3" s="7"/>
-      <c r="BJ3" s="7"/>
     </row>
   </sheetData>
   <phoneticPr fontId="0" type="noConversion"/>

</xml_diff>